<commit_message>
250828 revised for manuscript submission
submit to journal of polymer science
</commit_message>
<xml_diff>
--- a/result/AD/AD_after_removing_nBA_mechanism_oriented.xlsx
+++ b/result/AD/AD_after_removing_nBA_mechanism_oriented.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\81806\0_doctor_reserch\1_nitroxide\paper\sentence\github\result\AD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\81806\0_doctor_reserch\1_nitroxide\paper\250604_3rd_submit_M06\github\result\AD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E77B8C70-754B-4CDD-8157-6C20618EEFC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0B11676-CAF5-444C-AF09-C31FA0E2D3BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43095" yWindow="-2925" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -482,17 +482,12 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I20"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="3" max="3" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="11" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.15">
@@ -531,69 +526,69 @@
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2">
         <v>2.4500000000000002</v>
       </c>
       <c r="C2" s="2">
-        <v>2.3633294324852239</v>
-      </c>
-      <c r="D2" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2" t="b">
+        <v>2.0961665106451202</v>
+      </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" t="b">
         <v>1</v>
       </c>
       <c r="F2" s="2">
-        <v>1.936315150867258</v>
-      </c>
-      <c r="G2" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H2" s="2" t="b">
+        <v>2.1084035192395092</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" t="b">
         <v>1</v>
       </c>
       <c r="I2" s="2">
-        <v>2.3541255729342812</v>
-      </c>
-      <c r="J2" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="K2" s="2" t="b">
-        <v>0</v>
+        <v>1.7722407989949109</v>
+      </c>
+      <c r="J2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K2" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3">
         <v>1.8</v>
       </c>
       <c r="C3" s="2">
-        <v>2.618645806893352</v>
-      </c>
-      <c r="D3" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3" s="2" t="b">
+        <v>1.862913507931951</v>
+      </c>
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" t="b">
         <v>1</v>
       </c>
       <c r="F3" s="2">
-        <v>2.5018904397427022</v>
-      </c>
-      <c r="G3" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H3" s="2" t="b">
-        <v>1</v>
+        <v>1.7695547508653351</v>
+      </c>
+      <c r="G3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" t="b">
+        <v>0</v>
       </c>
       <c r="I3" s="2">
-        <v>1.691269947122815</v>
-      </c>
-      <c r="J3" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="K3" s="2" t="b">
+        <v>1.5771720485048191</v>
+      </c>
+      <c r="J3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3" t="b">
         <v>0</v>
       </c>
     </row>
@@ -601,69 +596,69 @@
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4">
         <v>2.0499999999999998</v>
       </c>
       <c r="C4" s="2">
-        <v>1.6488661857089459</v>
-      </c>
-      <c r="D4" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2" t="b">
+        <v>2.2434249789648359</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" t="b">
         <v>1</v>
       </c>
       <c r="F4" s="2">
-        <v>2.1196173234140749</v>
-      </c>
-      <c r="G4" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H4" s="2" t="b">
+        <v>2.235807665000757</v>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" t="b">
         <v>1</v>
       </c>
       <c r="I4" s="2">
-        <v>2.1477064574584022</v>
-      </c>
-      <c r="J4" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="K4" s="2" t="b">
-        <v>0</v>
+        <v>3.267510853901197</v>
+      </c>
+      <c r="J4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5">
         <v>1.9</v>
       </c>
       <c r="C5" s="2">
-        <v>1.521063376110829</v>
-      </c>
-      <c r="D5" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2" t="b">
-        <v>1</v>
+        <v>1.9591409231692141</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" t="b">
+        <v>0</v>
       </c>
       <c r="F5" s="2">
-        <v>1.337346034682511</v>
-      </c>
-      <c r="G5" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H5" s="2" t="b">
-        <v>0</v>
+        <v>1.8274054179770389</v>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" t="b">
+        <v>1</v>
       </c>
       <c r="I5" s="2">
-        <v>1.7221093080603509</v>
-      </c>
-      <c r="J5" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="K5" s="2" t="b">
+        <v>1.2326022356043469</v>
+      </c>
+      <c r="J5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5" t="b">
         <v>1</v>
       </c>
     </row>
@@ -671,34 +666,34 @@
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6">
         <v>1.75</v>
       </c>
       <c r="C6" s="2">
-        <v>2.1053832589550918</v>
-      </c>
-      <c r="D6" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2" t="b">
+        <v>1.8145435586165699</v>
+      </c>
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" t="b">
         <v>1</v>
       </c>
       <c r="F6" s="2">
-        <v>1.744469702228751</v>
-      </c>
-      <c r="G6" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H6" s="2" t="b">
+        <v>1.8731889123053611</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" t="b">
         <v>1</v>
       </c>
       <c r="I6" s="2">
-        <v>2.1639913159708639</v>
-      </c>
-      <c r="J6" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="K6" s="2" t="b">
+        <v>1.7709260654406529</v>
+      </c>
+      <c r="J6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" t="b">
         <v>1</v>
       </c>
     </row>
@@ -706,34 +701,34 @@
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7">
         <v>1.44</v>
       </c>
       <c r="C7" s="2">
-        <v>1.5852074148043791</v>
-      </c>
-      <c r="D7" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" s="2" t="b">
+        <v>1.478584277862792</v>
+      </c>
+      <c r="D7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" t="b">
         <v>1</v>
       </c>
       <c r="F7" s="2">
-        <v>1.539240478122218</v>
-      </c>
-      <c r="G7" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H7" s="2" t="b">
+        <v>1.504180754364276</v>
+      </c>
+      <c r="G7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" t="b">
         <v>1</v>
       </c>
       <c r="I7" s="2">
-        <v>1.4397952580856399</v>
-      </c>
-      <c r="J7" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="K7" s="2" t="b">
+        <v>1.5255981032995569</v>
+      </c>
+      <c r="J7" t="b">
+        <v>1</v>
+      </c>
+      <c r="K7" t="b">
         <v>1</v>
       </c>
     </row>
@@ -741,34 +736,34 @@
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8">
         <v>2.52</v>
       </c>
       <c r="C8" s="2">
-        <v>2.4352824557680841</v>
-      </c>
-      <c r="D8" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E8" s="2" t="b">
+        <v>2.1119208538279239</v>
+      </c>
+      <c r="D8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" t="b">
         <v>1</v>
       </c>
       <c r="F8" s="2">
-        <v>2.888950115459227</v>
-      </c>
-      <c r="G8" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H8" s="2" t="b">
+        <v>2.1993622831876731</v>
+      </c>
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" t="b">
         <v>1</v>
       </c>
       <c r="I8" s="2">
-        <v>3.902543033811861</v>
-      </c>
-      <c r="J8" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="K8" s="2" t="b">
+        <v>1.740837333490179</v>
+      </c>
+      <c r="J8" t="b">
+        <v>0</v>
+      </c>
+      <c r="K8" t="b">
         <v>0</v>
       </c>
     </row>
@@ -776,69 +771,69 @@
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9">
         <v>2.25</v>
       </c>
       <c r="C9" s="2">
-        <v>2.2467886040073468</v>
-      </c>
-      <c r="D9" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E9" s="2" t="b">
+        <v>2.5389185272360648</v>
+      </c>
+      <c r="D9" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" t="b">
         <v>1</v>
       </c>
       <c r="F9" s="2">
-        <v>2.2522111259568871</v>
-      </c>
-      <c r="G9" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H9" s="2" t="b">
+        <v>2.2288909544107178</v>
+      </c>
+      <c r="G9" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" t="b">
         <v>1</v>
       </c>
       <c r="I9" s="2">
-        <v>2.937668181104764</v>
-      </c>
-      <c r="J9" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="K9" s="2" t="b">
-        <v>1</v>
+        <v>1.8512700498079619</v>
+      </c>
+      <c r="J9" t="b">
+        <v>0</v>
+      </c>
+      <c r="K9" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10">
         <v>1.75</v>
       </c>
       <c r="C10" s="2">
-        <v>1.5561125320377731</v>
-      </c>
-      <c r="D10" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E10" s="2" t="b">
+        <v>1.6472446906242539</v>
+      </c>
+      <c r="D10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" t="b">
         <v>1</v>
       </c>
       <c r="F10" s="2">
-        <v>1.997818572987144</v>
-      </c>
-      <c r="G10" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H10" s="2" t="b">
+        <v>1.6831863633864219</v>
+      </c>
+      <c r="G10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" t="b">
         <v>1</v>
       </c>
       <c r="I10" s="2">
-        <v>1.571764408634488</v>
-      </c>
-      <c r="J10" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="K10" s="2" t="b">
+        <v>1.7116056570109031</v>
+      </c>
+      <c r="J10" t="b">
+        <v>1</v>
+      </c>
+      <c r="K10" t="b">
         <v>1</v>
       </c>
     </row>
@@ -846,104 +841,104 @@
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11">
         <v>3.81</v>
       </c>
       <c r="C11" s="2">
-        <v>1.9271910131973631</v>
-      </c>
-      <c r="D11" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E11" s="2" t="b">
+        <v>3.488344664639293</v>
+      </c>
+      <c r="D11" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" t="b">
         <v>1</v>
       </c>
       <c r="F11" s="2">
-        <v>2.519929788251841</v>
-      </c>
-      <c r="G11" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H11" s="2" t="b">
-        <v>1</v>
+        <v>3.6279989749300978</v>
+      </c>
+      <c r="G11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" t="b">
+        <v>0</v>
       </c>
       <c r="I11" s="2">
-        <v>1.9538691718487251</v>
-      </c>
-      <c r="J11" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="K11" s="2" t="b">
-        <v>1</v>
+        <v>3.5947204336654659</v>
+      </c>
+      <c r="J11" t="b">
+        <v>0</v>
+      </c>
+      <c r="K11" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12">
         <v>1.4</v>
       </c>
       <c r="C12" s="2">
-        <v>1.392839254217038</v>
-      </c>
-      <c r="D12" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E12" s="2" t="b">
-        <v>0</v>
+        <v>1.33749198639011</v>
+      </c>
+      <c r="D12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" t="b">
+        <v>1</v>
       </c>
       <c r="F12" s="2">
-        <v>1.3955306087143911</v>
-      </c>
-      <c r="G12" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H12" s="2" t="b">
+        <v>1.336200156734519</v>
+      </c>
+      <c r="G12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" t="b">
         <v>1</v>
       </c>
       <c r="I12" s="2">
-        <v>1.3999408880463839</v>
-      </c>
-      <c r="J12" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="K12" s="2" t="b">
-        <v>1</v>
+        <v>1.3596542692919431</v>
+      </c>
+      <c r="J12" t="b">
+        <v>0</v>
+      </c>
+      <c r="K12" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13">
         <v>1.45</v>
       </c>
       <c r="C13" s="2">
-        <v>1.8430435193117261</v>
-      </c>
-      <c r="D13" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E13" s="2" t="b">
+        <v>1.3920596827941041</v>
+      </c>
+      <c r="D13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" t="b">
         <v>1</v>
       </c>
       <c r="F13" s="2">
-        <v>1.452157020240791</v>
-      </c>
-      <c r="G13" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H13" s="2" t="b">
+        <v>1.4385703861571959</v>
+      </c>
+      <c r="G13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" t="b">
         <v>1</v>
       </c>
       <c r="I13" s="2">
-        <v>1.6091349197091149</v>
-      </c>
-      <c r="J13" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="K13" s="2" t="b">
+        <v>1.3654445101651029</v>
+      </c>
+      <c r="J13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K13" t="b">
         <v>1</v>
       </c>
     </row>
@@ -951,34 +946,34 @@
       <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14">
         <v>1.55</v>
       </c>
       <c r="C14" s="2">
-        <v>1.5844364591600111</v>
-      </c>
-      <c r="D14" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E14" s="2" t="b">
+        <v>1.449686990178642</v>
+      </c>
+      <c r="D14" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" t="b">
         <v>1</v>
       </c>
       <c r="F14" s="2">
-        <v>1.2386585491137569</v>
-      </c>
-      <c r="G14" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H14" s="2" t="b">
-        <v>1</v>
+        <v>1.34872096555984</v>
+      </c>
+      <c r="G14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14" t="b">
+        <v>0</v>
       </c>
       <c r="I14" s="2">
-        <v>1.3109228539415341</v>
-      </c>
-      <c r="J14" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="K14" s="2" t="b">
+        <v>1.2456754182348251</v>
+      </c>
+      <c r="J14" t="b">
+        <v>1</v>
+      </c>
+      <c r="K14" t="b">
         <v>1</v>
       </c>
     </row>
@@ -986,34 +981,34 @@
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15">
         <v>1.5</v>
       </c>
       <c r="C15" s="2">
-        <v>1.7591327281670239</v>
-      </c>
-      <c r="D15" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E15" s="2" t="b">
-        <v>1</v>
+        <v>1.688384642411102</v>
+      </c>
+      <c r="D15" t="b">
+        <v>0</v>
+      </c>
+      <c r="E15" t="b">
+        <v>0</v>
       </c>
       <c r="F15" s="2">
-        <v>1.5994077082420279</v>
-      </c>
-      <c r="G15" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H15" s="2" t="b">
-        <v>1</v>
+        <v>1.6376883713207151</v>
+      </c>
+      <c r="G15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" t="b">
+        <v>0</v>
       </c>
       <c r="I15" s="2">
-        <v>1.3377469428306841</v>
-      </c>
-      <c r="J15" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="K15" s="2" t="b">
+        <v>1.689480683485876</v>
+      </c>
+      <c r="J15" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1021,34 +1016,34 @@
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16">
         <v>1.55</v>
       </c>
       <c r="C16" s="2">
-        <v>1.6983680826101479</v>
-      </c>
-      <c r="D16" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E16" s="2" t="b">
-        <v>1</v>
+        <v>1.7848476912406639</v>
+      </c>
+      <c r="D16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E16" t="b">
+        <v>0</v>
       </c>
       <c r="F16" s="2">
-        <v>1.8772068917473239</v>
-      </c>
-      <c r="G16" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H16" s="2" t="b">
-        <v>1</v>
+        <v>1.933936227630134</v>
+      </c>
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" t="b">
+        <v>0</v>
       </c>
       <c r="I16" s="2">
-        <v>1.632581523740797</v>
-      </c>
-      <c r="J16" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="K16" s="2" t="b">
+        <v>1.730530514558603</v>
+      </c>
+      <c r="J16" t="b">
+        <v>0</v>
+      </c>
+      <c r="K16" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1056,34 +1051,34 @@
       <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17">
         <v>2.8</v>
       </c>
       <c r="C17" s="2">
-        <v>1.6586582210891521</v>
-      </c>
-      <c r="D17" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E17" s="2" t="b">
+        <v>2.588541758319185</v>
+      </c>
+      <c r="D17" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" t="b">
         <v>1</v>
       </c>
       <c r="F17" s="2">
-        <v>2.269604601896269</v>
-      </c>
-      <c r="G17" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H17" s="2" t="b">
+        <v>2.4771594706205859</v>
+      </c>
+      <c r="G17" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17" t="b">
         <v>1</v>
       </c>
       <c r="I17" s="2">
-        <v>1.9635349126193531</v>
-      </c>
-      <c r="J17" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="K17" s="2" t="b">
+        <v>2.710660477967584</v>
+      </c>
+      <c r="J17" t="b">
+        <v>1</v>
+      </c>
+      <c r="K17" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1091,104 +1086,104 @@
       <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18">
         <v>1.95</v>
       </c>
       <c r="C18" s="2">
-        <v>3.71979037513761</v>
-      </c>
-      <c r="D18" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E18" s="2" t="b">
+        <v>1.7830815058128371</v>
+      </c>
+      <c r="D18" t="b">
+        <v>1</v>
+      </c>
+      <c r="E18" t="b">
         <v>1</v>
       </c>
       <c r="F18" s="2">
-        <v>2.3173442293034339</v>
-      </c>
-      <c r="G18" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H18" s="2" t="b">
-        <v>1</v>
+        <v>2.0406761965820399</v>
+      </c>
+      <c r="G18" t="b">
+        <v>0</v>
+      </c>
+      <c r="H18" t="b">
+        <v>0</v>
       </c>
       <c r="I18" s="2">
-        <v>1.897174766057427</v>
-      </c>
-      <c r="J18" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="K18" s="2" t="b">
-        <v>1</v>
+        <v>1.985922682349234</v>
+      </c>
+      <c r="J18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K18" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19">
         <v>2.1</v>
       </c>
       <c r="C19" s="2">
-        <v>1.7122936059556639</v>
-      </c>
-      <c r="D19" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E19" s="2" t="b">
-        <v>1</v>
+        <v>1.2983160730849099</v>
+      </c>
+      <c r="D19" t="b">
+        <v>0</v>
+      </c>
+      <c r="E19" t="b">
+        <v>0</v>
       </c>
       <c r="F19" s="2">
-        <v>1.260577826366942</v>
-      </c>
-      <c r="G19" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H19" s="2" t="b">
+        <v>1.4939464214399301</v>
+      </c>
+      <c r="G19" t="b">
+        <v>0</v>
+      </c>
+      <c r="H19" t="b">
         <v>0</v>
       </c>
       <c r="I19" s="2">
-        <v>1.8259665432810659</v>
-      </c>
-      <c r="J19" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="K19" s="2" t="b">
-        <v>1</v>
+        <v>1.173326763208113</v>
+      </c>
+      <c r="J19" t="b">
+        <v>0</v>
+      </c>
+      <c r="K19" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20">
         <v>1.7</v>
       </c>
       <c r="C20" s="2">
-        <v>2.4070357672883032</v>
-      </c>
-      <c r="D20" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E20" s="2" t="b">
+        <v>1.548868149937223</v>
+      </c>
+      <c r="D20" t="b">
+        <v>1</v>
+      </c>
+      <c r="E20" t="b">
         <v>1</v>
       </c>
       <c r="F20" s="2">
-        <v>1.893135084934606</v>
-      </c>
-      <c r="G20" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H20" s="2" t="b">
+        <v>1.6116054082833311</v>
+      </c>
+      <c r="G20" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20" t="b">
         <v>1</v>
       </c>
       <c r="I20" s="2">
-        <v>1.6016644650892891</v>
-      </c>
-      <c r="J20" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="K20" s="2" t="b">
+        <v>1.792803181136549</v>
+      </c>
+      <c r="J20" t="b">
+        <v>1</v>
+      </c>
+      <c r="K20" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>